<commit_message>
chore: sync current work before merge
</commit_message>
<xml_diff>
--- a/boat_list.xlsx
+++ b/boat_list.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -687,22 +687,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>인천</t>
+          <t>화성</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>영흥항</t>
+          <t>전곡항</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>팀만수호</t>
+          <t>명성호</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://teammansu.kr/index.php?mid=bk</t>
+          <t>http://xn--hq1b31ko5fzpfdsxrtb.com/index.php?mid=bk</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
@@ -713,22 +713,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>군산</t>
+          <t>인천</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>비응항</t>
+          <t>영흥항</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>샤크호 선단</t>
+          <t>팀만수호</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://sharkho.sunsang24.com/ship/schedule_fleet/</t>
+          <t>https://teammansu.kr/index.php?mid=bk</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -739,22 +739,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>화성</t>
+          <t>군산</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>전곡항</t>
+          <t>비응항</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>신명호 선단</t>
+          <t>샤크호 선단</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>http://www.shinmyungho.com/index.php?mid=bk</t>
+          <t>https://sharkho.sunsang24.com/ship/schedule_fleet/</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
@@ -765,29 +765,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>격포</t>
+          <t>화성</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>격포항</t>
+          <t>전곡항</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>변산레저낚시</t>
+          <t>신명호 선단</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://banak24.com/index.php?mid=bk</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>카이저3호 문어만 이용 좋음</t>
-        </is>
-      </c>
+          <t>http://www.shinmyungho.com/index.php?mid=bk</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -795,25 +791,29 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>군산</t>
+          <t>격포</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>비응항</t>
+          <t>격포항</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>엘리스호</t>
+          <t>변산레저낚시</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://alice.sunsang24.com/ship/schedule_fleet/</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
+          <t>https://banak24.com/index.php?mid=bk</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>카이저3호 문어만 이용 좋음</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -821,22 +821,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>보령</t>
+          <t>군산</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>홍원항</t>
+          <t>비응항</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>뉴해양호</t>
+          <t>엘리스호</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://newhaeyang.sunsang24.com/ship/schedule_fleet/</t>
+          <t>https://alice.sunsang24.com/ship/schedule_fleet/</t>
         </is>
       </c>
       <c r="F15" t="inlineStr"/>
@@ -857,20 +857,15 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>조커호</t>
+          <t>뉴해양호</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>http://seasidefishing.kr/index.php?mid=bk</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BDJ 추천 배, 선장 젊고, 열정 많음
-</t>
-        </is>
-      </c>
+          <t>https://newhaeyang.sunsang24.com/ship/schedule_fleet/</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -883,17 +878,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>대천항</t>
+          <t>홍원항</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>팀루피호</t>
+          <t>조커호</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://masterfishing.kr/index.php?mid=bk</t>
+          <t>http://seasidefishing.kr/index.php?mid=bk</t>
         </is>
       </c>
       <c r="F17" t="inlineStr"/>
@@ -909,20 +904,24 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>구매항</t>
+          <t>대천항</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>악바리호</t>
+          <t>팀루피호</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://akbari.sunsang24.com/ship/schedule_fleet/</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
+          <t>https://masterfishing.kr/index.php?mid=bk</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>BDJ 추천 배, 선장 젊고, 열정 많음</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -935,17 +934,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>오천항</t>
+          <t>구매항</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>범블비호</t>
+          <t>악바리호</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>http://xn--xk3bm1aee249g.com/index.php?mid=bk</t>
+          <t>https://akbari.sunsang24.com/ship/schedule_fleet/</t>
         </is>
       </c>
       <c r="F19" t="inlineStr"/>
@@ -966,19 +965,15 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>루키호</t>
+          <t>범블비호</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>http://www.yamujinfishing.com/index.php?mid=bk</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>오천에 유명 배</t>
-        </is>
-      </c>
+          <t>http://xn--xk3bm1aee249g.com/index.php?mid=bk</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -996,17 +991,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>프랜드피싱</t>
+          <t>루키호</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>http://www.friendho.com/index.php?mid=bk</t>
+          <t>http://www.yamujinfishing.com/index.php?mid=bk</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>멘구전문 갑,쭈 잘함</t>
+          <t>오천에 유명 배</t>
         </is>
       </c>
     </row>
@@ -1016,27 +1011,27 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>태안</t>
+          <t>보령</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>마검포항</t>
+          <t>오천항</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>가가호</t>
+          <t>프랜드피싱</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://gagaho.sunsang24.com/ship/schedule_fleet/</t>
+          <t>http://www.friendho.com/index.php?mid=bk</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>내꼬야,유튜브가 주로 이용, 갑잘함</t>
+          <t>멘구전문 갑,쭈 잘함</t>
         </is>
       </c>
     </row>
@@ -1056,15 +1051,19 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>뉴정원호</t>
+          <t>가가호</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://www.jungwonho.com/index.php?mid=bk</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
+          <t>https://gagaho.sunsang24.com/ship/schedule_fleet/</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>내꼬야,유튜브가 주로 이용, 갑잘함</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1082,12 +1081,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>만선호</t>
+          <t>뉴정원호</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://mansunho.sunsang24.com/ship/schedule_fleet/</t>
+          <t>https://www.jungwonho.com/index.php?mid=bk</t>
         </is>
       </c>
       <c r="F24" t="inlineStr"/>
@@ -1103,17 +1102,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>영목항</t>
+          <t>마검포항</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>카라호</t>
+          <t>만선호</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://karaho.kr/index.php?mid=bk</t>
+          <t>https://mansunho.sunsang24.com/ship/schedule_fleet/</t>
         </is>
       </c>
       <c r="F25" t="inlineStr"/>
@@ -1134,19 +1133,15 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>청광호</t>
+          <t>카라호</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>http://www.chungkwangho.net/index.php?mid=bk</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>우럭귀신 자주 이용하는 배</t>
-        </is>
-      </c>
+          <t>https://karaho.kr/index.php?mid=bk</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1154,27 +1149,27 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>당진</t>
+          <t>태안</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>장고항</t>
+          <t>영목항</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>디스커버리호</t>
+          <t>청광호</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>http://www.discoveryho.net/index.php?mid=bk</t>
+          <t>http://www.chungkwangho.net/index.php?mid=bk</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>김조사, 송조사 추천, 꼬리쪽 잘함</t>
+          <t>우럭귀신 자주 이용하는 배</t>
         </is>
       </c>
     </row>
@@ -1184,25 +1179,29 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>안산</t>
+          <t>당진</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>오이도항</t>
+          <t>장고항</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>포세이돈호</t>
+          <t>디스커버리호</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://poseidon.sunsang24.com/ship/schedule_fleet/</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr"/>
+          <t>http://www.discoveryho.net/index.php?mid=bk</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>김조사, 송조사 추천, 꼬리쪽 잘함</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1210,22 +1209,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>인천</t>
+          <t>안산</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>영흥항</t>
+          <t>오이도항</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>금강7호</t>
+          <t>포세이돈호</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>http://www.kumkangho.co.kr/index.php?mid=bk</t>
+          <t>https://poseidon.sunsang24.com/ship/schedule_fleet/</t>
         </is>
       </c>
       <c r="F29" t="inlineStr"/>
@@ -1236,22 +1235,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>여수</t>
+          <t>인천</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>국동항</t>
+          <t>영흥항</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>트윈스타</t>
+          <t>금강7호</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://twin.sunsang24.com/ship/schedule_fleet/</t>
+          <t>http://www.kumkangho.co.kr/index.php?mid=bk</t>
         </is>
       </c>
       <c r="F30" t="inlineStr"/>
@@ -1272,12 +1271,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>만진스타호</t>
+          <t>트윈스타</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://manjinstar.sunsang24.com/ship/schedule_fleet/</t>
+          <t>https://twin.sunsang24.com/ship/schedule_fleet/</t>
         </is>
       </c>
       <c r="F31" t="inlineStr"/>
@@ -1298,12 +1297,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>오션스타호</t>
+          <t>만진스타호</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://ysoceanstar.sunsang24.com/ship/schedule_fleet</t>
+          <t>https://manjinstar.sunsang24.com/ship/schedule_fleet/</t>
         </is>
       </c>
       <c r="F32" t="inlineStr"/>
@@ -1319,17 +1318,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>종포항</t>
+          <t>국동항</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>빅보스호</t>
+          <t>오션스타호</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://big.sunsang24.com/ship/schedule_fleet/</t>
+          <t>https://ysoceanstar.sunsang24.com/ship/schedule_fleet</t>
         </is>
       </c>
       <c r="F33" t="inlineStr"/>
@@ -1345,17 +1344,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>국동항</t>
+          <t>종포항</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>써니호</t>
+          <t>빅보스호</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://sunny.sunsang24.com/ship/schedule_fleet/</t>
+          <t>https://big.sunsang24.com/ship/schedule_fleet/</t>
         </is>
       </c>
       <c r="F34" t="inlineStr"/>
@@ -1366,22 +1365,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>고흥</t>
+          <t>여수</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>녹동방파제</t>
+          <t>국동항</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>빅원호</t>
+          <t>써니호</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://bigone.sunsang24.com/ship/schedule_fleet/</t>
+          <t>https://sunny.sunsang24.com/ship/schedule_fleet/</t>
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
@@ -1402,19 +1401,15 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>에이스호</t>
+          <t>빅원호</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://aceho.sunsang24.com/ship/schedule_fleet/</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>신조선, 선장 배질 잘함,깨끗함</t>
-        </is>
-      </c>
+          <t>https://bigone.sunsang24.com/ship/schedule_fleet/</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1422,25 +1417,29 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>여수</t>
+          <t>고흥</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>신추항</t>
+          <t>녹동방파제</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>그린나래</t>
+          <t>에이스호</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://green.sunsang24.com/ship/schedule_fleet/</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr"/>
+          <t>https://aceho.sunsang24.com/ship/schedule_fleet/</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>신조선, 선장 배질 잘함,깨끗함</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1448,22 +1447,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>서산</t>
+          <t>여수</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>삼길포항</t>
+          <t>신추항</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>만석낚시 선단</t>
+          <t>그린나래</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>http://www.mscufishing.com/index.php?mid=bk</t>
+          <t>https://green.sunsang24.com/ship/schedule_fleet/</t>
         </is>
       </c>
       <c r="F38" t="inlineStr"/>
@@ -1474,29 +1473,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>여수</t>
+          <t>서산</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>돌산항</t>
+          <t>삼길포항</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>영심이호</t>
+          <t>만석낚시 선단</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://0simi.sunsang24.com/ship/schedule_fleet/</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>전투 낚시 전문, 배는 작지만, 선장 마인드 좋음</t>
-        </is>
-      </c>
+          <t>http://www.mscufishing.com/index.php?mid=bk</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1504,25 +1499,29 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>인천</t>
+          <t>여수</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>영흥항</t>
+          <t>돌산항</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>만수피싱</t>
+          <t>영심이호</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://teammansu.kr/index.php?mid=bk</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr"/>
+          <t>https://0simi.sunsang24.com/ship/schedule_fleet/</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>전투 낚시 전문, 배는 작지만, 선장 마인드 좋음</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -1530,22 +1529,22 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>보령</t>
+          <t>인천</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>남당항</t>
+          <t>영흥항</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>은가비호</t>
+          <t>만수피싱</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://eungabi.sunsang24.com/ship/schedule_fleet/</t>
+          <t>https://teammansu.kr/index.php?mid=bk</t>
         </is>
       </c>
       <c r="F41" t="inlineStr"/>
@@ -1556,22 +1555,22 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>서산</t>
+          <t>보령</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>삼길포항</t>
+          <t>남당항</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>헤르메스호</t>
+          <t>은가비호</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>http://hermes.thefishing.kr/index.php?mid=bk</t>
+          <t>https://eungabi.sunsang24.com/ship/schedule_fleet/</t>
         </is>
       </c>
       <c r="F42" t="inlineStr"/>
@@ -1582,22 +1581,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>평택</t>
+          <t>서산</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>평택항</t>
+          <t>삼길포항</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>수복호</t>
+          <t>헤르메스호</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://subokho.sunsang24.com/ship/schedule_fleet/</t>
+          <t>http://hermes.thefishing.kr/index.php?mid=bk</t>
         </is>
       </c>
       <c r="F43" t="inlineStr"/>
@@ -1608,22 +1607,22 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>태안</t>
+          <t>평택</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>모항항</t>
+          <t>평택항</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>라온피싱</t>
+          <t>수복호</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>http://raonfishing.com/index.php?mid=bk</t>
+          <t>https://subokho.sunsang24.com/ship/schedule_fleet/</t>
         </is>
       </c>
       <c r="F44" t="inlineStr"/>
@@ -1634,22 +1633,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>고흥</t>
+          <t>태안</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>녹동방파제</t>
+          <t>모항항</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>몬스터호</t>
+          <t>라온피싱</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>https://mon.sunsang24.com/ship/schedule_fleet/</t>
+          <t>http://raonfishing.com/index.php?mid=bk</t>
         </is>
       </c>
       <c r="F45" t="inlineStr"/>
@@ -1670,12 +1669,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>여명호</t>
+          <t>몬스터호</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>https://ym.sunsang24.com/ship/schedule_fleet/</t>
+          <t>https://mon.sunsang24.com/ship/schedule_fleet/</t>
         </is>
       </c>
       <c r="F46" t="inlineStr"/>
@@ -1686,25 +1685,81 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
+          <t>고흥</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>녹동방파제</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>여명호</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>https://ym.sunsang24.com/ship/schedule_fleet/</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
           <t>여수</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>돌산항</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>청홍낚시</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>https://chf.sunsang24.com/ship/schedule_fleet/</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr"/>
+      <c r="F48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>여수</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>국동항</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>블랙펄호</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>https://ysblackpearl.sunsang24.com/ship/schedule_fleet/</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>멘구 추천 문어 선사</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>